<commit_message>
OK, now I think all the formant knobs are right - just 0..255 works best!
</commit_message>
<xml_diff>
--- a/Pins_Notes_Tables.xlsx
+++ b/Pins_Notes_Tables.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Propeller Pins" sheetId="3" r:id="rId1"/>
     <sheet name="frequency table" sheetId="4" r:id="rId2"/>
     <sheet name="LCDViews" sheetId="5" r:id="rId3"/>
+    <sheet name="formant values" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'frequency table'!$A$1:$F$62</definedName>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="192">
   <si>
     <t>Frequency (Hz)</t>
   </si>
@@ -2447,6 +2448,54 @@
   </si>
   <si>
     <t>P32</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>ee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    oh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   foot</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> boot</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    uh</t>
+  </si>
+  <si>
+    <t>f1</t>
+  </si>
+  <si>
+    <t>f2</t>
+  </si>
+  <si>
+    <t>f3</t>
+  </si>
+  <si>
+    <t>f4</t>
   </si>
 </sst>
 </file>
@@ -2597,7 +2646,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2643,6 +2692,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2947,7 +3002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -5427,4 +5482,318 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:Q29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12:C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>9.5</v>
+      </c>
+      <c r="D3">
+        <v>19</v>
+      </c>
+      <c r="E3">
+        <f>256/36</f>
+        <v>7.1111111111111107</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D6" s="19" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>450</v>
+      </c>
+      <c r="C7" s="9">
+        <f>(B7+$C$3)/$D$3</f>
+        <v>24.184210526315791</v>
+      </c>
+      <c r="D7" s="20">
+        <f>C7/7</f>
+        <v>3.4548872180451129</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>2060</v>
+      </c>
+      <c r="C8" s="9">
+        <f t="shared" ref="C8:C10" si="0">(B8+$C$3)/$D$3</f>
+        <v>108.92105263157895</v>
+      </c>
+      <c r="D8" s="20">
+        <f t="shared" ref="D8:D10" si="1">C8/7</f>
+        <v>15.56015037593985</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>2700</v>
+      </c>
+      <c r="C9" s="9">
+        <f t="shared" si="0"/>
+        <v>142.60526315789474</v>
+      </c>
+      <c r="D9" s="20">
+        <f t="shared" si="1"/>
+        <v>20.372180451127821</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>3570</v>
+      </c>
+      <c r="C10" s="9">
+        <f t="shared" si="0"/>
+        <v>188.39473684210526</v>
+      </c>
+      <c r="D10" s="20">
+        <f t="shared" si="1"/>
+        <v>26.913533834586467</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="20">
+        <v>2.1766917293233083</v>
+      </c>
+      <c r="C13" s="9">
+        <v>3.4548872180451129</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="20">
+        <v>15.409774436090226</v>
+      </c>
+      <c r="C14" s="9">
+        <v>15.56015037593985</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="20">
+        <v>22.928571428571427</v>
+      </c>
+      <c r="C15" s="9">
+        <v>20.372180451127821</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="20">
+        <v>27.139097744360903</v>
+      </c>
+      <c r="C16" s="9">
+        <v>26.913533834586467</v>
+      </c>
+    </row>
+    <row r="25" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="G25" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="H25" s="19" t="s">
+        <v>178</v>
+      </c>
+      <c r="I25" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="J25" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="K25" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="L25" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="M25" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="N25" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="O25" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="P25" s="19" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q25" s="19" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="26" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F26" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="G26">
+        <v>280</v>
+      </c>
+      <c r="H26">
+        <v>450</v>
+      </c>
+      <c r="I26">
+        <v>550</v>
+      </c>
+      <c r="J26">
+        <v>700</v>
+      </c>
+      <c r="K26">
+        <v>775</v>
+      </c>
+      <c r="L26">
+        <v>575</v>
+      </c>
+      <c r="M26">
+        <v>425</v>
+      </c>
+      <c r="N26">
+        <v>275</v>
+      </c>
+      <c r="O26">
+        <v>560</v>
+      </c>
+      <c r="P26">
+        <v>560</v>
+      </c>
+      <c r="Q26">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="27" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F27" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="G27">
+        <v>2040</v>
+      </c>
+      <c r="H27">
+        <v>2060</v>
+      </c>
+      <c r="I27">
+        <v>1950</v>
+      </c>
+      <c r="J27">
+        <v>1800</v>
+      </c>
+      <c r="K27">
+        <v>1100</v>
+      </c>
+      <c r="L27">
+        <v>900</v>
+      </c>
+      <c r="M27">
+        <v>1000</v>
+      </c>
+      <c r="N27">
+        <v>850</v>
+      </c>
+      <c r="O27">
+        <v>1200</v>
+      </c>
+      <c r="P27">
+        <v>820</v>
+      </c>
+      <c r="Q27">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="28" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F28" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="G28">
+        <v>3040</v>
+      </c>
+      <c r="H28">
+        <v>2700</v>
+      </c>
+      <c r="I28">
+        <v>2600</v>
+      </c>
+      <c r="J28">
+        <v>2550</v>
+      </c>
+      <c r="K28">
+        <v>2500</v>
+      </c>
+      <c r="L28">
+        <v>2450</v>
+      </c>
+      <c r="M28">
+        <v>2400</v>
+      </c>
+      <c r="N28">
+        <v>2400</v>
+      </c>
+      <c r="O28">
+        <v>1500</v>
+      </c>
+      <c r="P28">
+        <v>2700</v>
+      </c>
+      <c r="Q28">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="29" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F29" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="G29">
+        <v>3600</v>
+      </c>
+      <c r="H29">
+        <v>3570</v>
+      </c>
+      <c r="I29">
+        <v>3400</v>
+      </c>
+      <c r="J29">
+        <v>3400</v>
+      </c>
+      <c r="K29">
+        <v>3500</v>
+      </c>
+      <c r="L29">
+        <v>3500</v>
+      </c>
+      <c r="M29">
+        <v>3500</v>
+      </c>
+      <c r="N29">
+        <v>3500</v>
+      </c>
+      <c r="O29">
+        <v>3050</v>
+      </c>
+      <c r="P29">
+        <v>3600</v>
+      </c>
+      <c r="Q29">
+        <v>3100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
physically removed the LCD, physically added a 3 toggle "mode" switch. Only 1 of the two parts of the switch are working, so it is only two state at this time Everything works. Updated most of the pins in the xl spreadsheet
</commit_message>
<xml_diff>
--- a/Pins_Notes_Tables.xlsx
+++ b/Pins_Notes_Tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035"/>
   </bookViews>
   <sheets>
     <sheet name="Propeller Pins" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="209">
   <si>
     <t>Frequency (Hz)</t>
   </si>
@@ -2496,13 +2496,64 @@
   </si>
   <si>
     <t>f4</t>
+  </si>
+  <si>
+    <t>CS_PIN</t>
+  </si>
+  <si>
+    <t>DATA_PIN</t>
+  </si>
+  <si>
+    <t>ADDRESS</t>
+  </si>
+  <si>
+    <t>IO_CLOCK</t>
+  </si>
+  <si>
+    <t>CLK_PIN</t>
+  </si>
+  <si>
+    <t>'*** adc ***</t>
+  </si>
+  <si>
+    <t>MODE_S1</t>
+  </si>
+  <si>
+    <t>MODE_S2</t>
+  </si>
+  <si>
+    <t>'*** mode ***</t>
+  </si>
+  <si>
+    <t>Keyboard Input</t>
+  </si>
+  <si>
+    <t>Keyboard Output</t>
+  </si>
+  <si>
+    <t>Keyboard_Quadrant_Index</t>
+  </si>
+  <si>
+    <t>Keyboard_Key_Index</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>reserved</t>
+  </si>
+  <si>
+    <t>LCD_Line</t>
+  </si>
+  <si>
+    <t>lcd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2566,6 +2617,14 @@
       <b/>
       <sz val="12"/>
       <color theme="8" tint="0.79998168889431442"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2646,7 +2705,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2698,6 +2757,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3000,19 +3060,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>140</v>
       </c>
@@ -3022,170 +3084,305 @@
       <c r="C1" s="18" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="18" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>201</v>
+      </c>
+      <c r="D4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>201</v>
+      </c>
+      <c r="D7" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>201</v>
+      </c>
+      <c r="D8" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>201</v>
+      </c>
+      <c r="D9" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>196</v>
+      </c>
+      <c r="D15" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>202</v>
+      </c>
+      <c r="D16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>202</v>
+      </c>
+      <c r="D17" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>202</v>
+      </c>
+      <c r="D18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>202</v>
+      </c>
+      <c r="D23" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>202</v>
+      </c>
+      <c r="D24" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>195</v>
+      </c>
+      <c r="D25" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>194</v>
+      </c>
+      <c r="D26" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>193</v>
+      </c>
+      <c r="D27" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>192</v>
+      </c>
+      <c r="D28" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>198</v>
+      </c>
+      <c r="D29" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>199</v>
+      </c>
+      <c r="D30" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>175</v>
+      </c>
+      <c r="C34" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -5488,7 +5685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12:C16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
got the 3-way mode switch working.  Switched from pull-down to pull-up resistors to get the switch functioning and adjusted the logic accordingly.
</commit_message>
<xml_diff>
--- a/Pins_Notes_Tables.xlsx
+++ b/Pins_Notes_Tables.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="212">
   <si>
     <t>Frequency (Hz)</t>
   </si>
@@ -2547,6 +2547,15 @@
   </si>
   <si>
     <t>lcd</t>
+  </si>
+  <si>
+    <t>RIGHT_STEREO_PIN</t>
+  </si>
+  <si>
+    <t>LEFT_STEREO_PIN</t>
+  </si>
+  <si>
+    <t>stereo out</t>
   </si>
 </sst>
 </file>
@@ -3064,7 +3073,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3190,10 +3199,22 @@
       <c r="B12" t="s">
         <v>153</v>
       </c>
+      <c r="C12" t="s">
+        <v>209</v>
+      </c>
+      <c r="D12" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>154</v>
+      </c>
+      <c r="C13" t="s">
+        <v>210</v>
+      </c>
+      <c r="D13" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added 'notes' on word formation
</commit_message>
<xml_diff>
--- a/Pins_Notes_Tables.xlsx
+++ b/Pins_Notes_Tables.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Propeller Pins" sheetId="3" r:id="rId1"/>
     <sheet name="frequency table" sheetId="4" r:id="rId2"/>
     <sheet name="LCDViews" sheetId="5" r:id="rId3"/>
     <sheet name="formant values" sheetId="7" r:id="rId4"/>
+    <sheet name="word values" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'frequency table'!$A$1:$F$62</definedName>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="219">
   <si>
     <t>Frequency (Hz)</t>
   </si>
@@ -2556,6 +2557,27 @@
   </si>
   <si>
     <t>stereo out</t>
+  </si>
+  <si>
+    <t>knob</t>
+  </si>
+  <si>
+    <t>~255</t>
+  </si>
+  <si>
+    <t>~10</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>up to max</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>"YeahOohh"</t>
   </si>
 </sst>
 </file>
@@ -2772,7 +2794,31 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2780,6 +2826,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:C22" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A2:C22"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Column1"/>
+    <tableColumn id="2" name="up to max"/>
+    <tableColumn id="3" name="decimal"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3071,7 +3129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
@@ -6014,4 +6072,262 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>44</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>58</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>76</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>188</v>
+      </c>
+      <c r="C7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>58</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>42</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>130</v>
+      </c>
+      <c r="C10">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>74</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>123</v>
+      </c>
+      <c r="C13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>57</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>126</v>
+      </c>
+      <c r="C15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>85</v>
+      </c>
+      <c r="C17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>65</v>
+      </c>
+      <c r="C18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>57</v>
+      </c>
+      <c r="C19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>17</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>